<commit_message>
add logger & .bat files
</commit_message>
<xml_diff>
--- a/IF_Input.xlsx
+++ b/IF_Input.xlsx
@@ -8,26 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuan.nguyen\Projects\rwsif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34056278-01CF-4436-B162-F3C45CE359B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8104D75-692F-4BCE-8002-DFB9CD86FCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="738" activeTab="4" xr2:uid="{D97CDD91-3225-4036-A94C-C727C1F15EC9}"/>
+    <workbookView xWindow="5760" yWindow="3408" windowWidth="17280" windowHeight="8832" tabRatio="738" xr2:uid="{D97CDD91-3225-4036-A94C-C727C1F15EC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="odh2" sheetId="2" r:id="rId1"/>
-    <sheet name="odh" sheetId="9" r:id="rId2"/>
-    <sheet name="odl" sheetId="4" r:id="rId3"/>
-    <sheet name="pah" sheetId="6" r:id="rId4"/>
-    <sheet name="pal" sheetId="8" r:id="rId5"/>
-    <sheet name="odh_guide" sheetId="1" r:id="rId6"/>
-    <sheet name="odl_guide" sheetId="3" r:id="rId7"/>
-    <sheet name="pah_guide" sheetId="5" r:id="rId8"/>
-    <sheet name="pal_guide" sheetId="7" r:id="rId9"/>
+    <sheet name="odh" sheetId="2" r:id="rId1"/>
+    <sheet name="odl" sheetId="4" r:id="rId2"/>
+    <sheet name="pah" sheetId="6" r:id="rId3"/>
+    <sheet name="pal" sheetId="8" r:id="rId4"/>
+    <sheet name="odh_guide" sheetId="1" r:id="rId5"/>
+    <sheet name="odl_guide" sheetId="3" r:id="rId6"/>
+    <sheet name="pah_guide" sheetId="5" r:id="rId7"/>
+    <sheet name="pal_guide" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">odh_guide!$A$1:$E$197</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">odl_guide!$A$1:$E$89</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">pah_guide!$A$1:$E$75</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">pal_guide!$A$1:$E$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">odh_guide!$A$1:$E$197</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">odl_guide!$A$1:$E$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">pah_guide!$A$1:$E$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">pal_guide!$A$1:$E$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="367">
   <si>
     <t>Name</t>
   </si>
@@ -1023,22 +1022,10 @@
     <t>Expected_Gross_Weight</t>
   </si>
   <si>
-    <t>REPACK</t>
-  </si>
-  <si>
-    <t>cp</t>
-  </si>
-  <si>
-    <t>rpk</t>
-  </si>
-  <si>
     <t>PAH</t>
   </si>
   <si>
     <t>250617COPIA-ECOLAB</t>
-  </si>
-  <si>
-    <t>20250620000000</t>
   </si>
   <si>
     <t>PAL</t>
@@ -1160,6 +1147,12 @@
   </si>
   <si>
     <t xml:space="preserve"> VN40010008 </t>
+  </si>
+  <si>
+    <t>20250620000000</t>
+  </si>
+  <si>
+    <t>PAD</t>
   </si>
 </sst>
 </file>
@@ -1573,10 +1566,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CD735A-45CF-42CA-99A7-17D71D0664B8}">
-  <dimension ref="A1:I3"/>
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1589,10 +1585,9 @@
     <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.44140625" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1617,11 +1612,8 @@
       <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>223</v>
       </c>
@@ -1647,7 +1639,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>223</v>
       </c>
@@ -1679,688 +1671,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB92746-E6FA-484E-9E2A-47B7397C38FC}">
-  <dimension ref="A1:GN3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:196">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="BG1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="BH1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BI1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="BJ1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="BL1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="BN1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="BO1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BP1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="BW1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="BX1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="BY1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="BZ1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="CA1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="CB1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="CC1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="CD1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="CE1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="CF1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="CG1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="CH1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="CI1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="CJ1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="CK1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="CL1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="CM1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="CN1" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="CO1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="CP1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="CQ1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="CR1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="CS1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="CT1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="CU1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="CV1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="CW1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="CX1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="CY1" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="CZ1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="DA1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="DB1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="DC1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="DD1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="DE1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="DF1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="DG1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="DH1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="DI1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="DJ1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="DK1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="DL1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="DM1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="DN1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="DO1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="DP1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="DQ1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="DR1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="DT1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="DU1" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="DV1" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="DW1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="DX1" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="DY1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="DZ1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="EA1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="EB1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="EC1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="ED1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="EE1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="EF1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="EG1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="EH1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="EI1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="EJ1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="EK1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="EL1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="EM1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="EN1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="EO1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="EP1" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="EQ1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="ER1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="ES1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="ET1" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="EU1" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="EV1" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="EW1" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="EX1" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="EY1" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="EZ1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="FA1" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="FB1" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="FC1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="FD1" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="FE1" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="FF1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="FG1" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="FH1" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="FI1" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="FJ1" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="FK1" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="FL1" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="FM1" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="FN1" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="FO1" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="FP1" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="FQ1" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="FR1" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="FS1" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="FT1" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="FU1" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="FV1" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="FW1" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="FX1" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="FY1" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="FZ1" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="GA1" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="GB1" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="GC1" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="GD1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="GE1" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="GF1" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="GG1" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="GH1" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="GI1" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="GJ1" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="GK1" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="GL1" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="GM1" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="GN1" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:196">
-      <c r="A2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G2" t="s">
-        <v>227</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>228</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>228</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>324</v>
-      </c>
-      <c r="GL2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:196">
-      <c r="A3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" t="s">
-        <v>284</v>
-      </c>
-      <c r="G3" t="s">
-        <v>227</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>229</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>229</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>323</v>
-      </c>
-      <c r="DH3" t="s">
-        <v>325</v>
-      </c>
-      <c r="GL3">
-        <v>456</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61B5B39-9828-49D8-BED8-5980F93DA4E7}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2409,12 +1727,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3A9925-7AFF-42EB-AA45-3D9B84782C8A}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2450,13 +1771,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B2" t="s">
         <v>224</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D2" t="s">
         <v>228</v>
@@ -2468,7 +1789,7 @@
         <v>228</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>328</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -2476,12 +1797,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C330B358-1262-4847-9536-D5EEEE3F24C6}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2531,16 +1855,16 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s">
         <v>224</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E2" s="7">
         <v>3</v>
@@ -2552,27 +1876,27 @@
         <v>228</v>
       </c>
       <c r="H2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="J2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B3" t="s">
         <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E3" s="7">
         <v>2</v>
@@ -2584,27 +1908,27 @@
         <v>228</v>
       </c>
       <c r="H3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="J3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B4" t="s">
         <v>224</v>
       </c>
       <c r="C4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D4" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E4" s="7">
         <v>14</v>
@@ -2616,27 +1940,27 @@
         <v>228</v>
       </c>
       <c r="H4" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B5" t="s">
         <v>224</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D5" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E5" s="7">
         <v>7</v>
@@ -2648,27 +1972,27 @@
         <v>228</v>
       </c>
       <c r="H5" t="s">
+        <v>344</v>
+      </c>
+      <c r="I5" t="s">
         <v>348</v>
       </c>
-      <c r="I5" t="s">
-        <v>352</v>
-      </c>
       <c r="J5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B6" t="s">
         <v>224</v>
       </c>
       <c r="C6" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E6" s="7">
         <v>4</v>
@@ -2680,27 +2004,27 @@
         <v>228</v>
       </c>
       <c r="H6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I6" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="J6" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>329</v>
+        <v>366</v>
       </c>
       <c r="B7" t="s">
         <v>224</v>
       </c>
       <c r="C7" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
@@ -2712,27 +2036,27 @@
         <v>228</v>
       </c>
       <c r="H7" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="J7" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B8" t="s">
         <v>224</v>
       </c>
       <c r="C8" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D8" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E8" s="7">
         <v>9</v>
@@ -2744,27 +2068,27 @@
         <v>228</v>
       </c>
       <c r="H8" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I8" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B9" t="s">
         <v>224</v>
       </c>
       <c r="C9" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D9" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E9" s="7">
         <v>3</v>
@@ -2776,27 +2100,27 @@
         <v>228</v>
       </c>
       <c r="H9" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="J9" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B10" t="s">
         <v>224</v>
       </c>
       <c r="C10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D10" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E10" s="7">
         <v>3</v>
@@ -2808,27 +2132,27 @@
         <v>228</v>
       </c>
       <c r="H10" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I10" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="J10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B11" t="s">
         <v>224</v>
       </c>
       <c r="C11" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D11" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E11" s="7">
         <v>4</v>
@@ -2840,27 +2164,27 @@
         <v>228</v>
       </c>
       <c r="H11" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B12" t="s">
         <v>224</v>
       </c>
       <c r="C12" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D12" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E12" s="7">
         <v>4</v>
@@ -2872,27 +2196,27 @@
         <v>228</v>
       </c>
       <c r="H12" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I12" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J12" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B13" t="s">
         <v>224</v>
       </c>
       <c r="C13" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D13" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
@@ -2904,27 +2228,27 @@
         <v>228</v>
       </c>
       <c r="H13" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I13" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="J13" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B14" t="s">
         <v>224</v>
       </c>
       <c r="C14" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D14" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E14" s="7">
         <v>4</v>
@@ -2936,27 +2260,27 @@
         <v>228</v>
       </c>
       <c r="H14" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I14" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J14" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B15" t="s">
         <v>224</v>
       </c>
       <c r="C15" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D15" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E15" s="7">
         <v>4</v>
@@ -2968,27 +2292,27 @@
         <v>228</v>
       </c>
       <c r="H15" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I15" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J15" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B16" t="s">
         <v>224</v>
       </c>
       <c r="C16" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D16" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E16" s="7">
         <v>4</v>
@@ -3000,27 +2324,27 @@
         <v>228</v>
       </c>
       <c r="H16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I16" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B17" t="s">
         <v>224</v>
       </c>
       <c r="C17" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D17" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E17" s="7">
         <v>4</v>
@@ -3032,13 +2356,13 @@
         <v>228</v>
       </c>
       <c r="H17" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I17" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J17" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -3046,12 +2370,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD304A0-4224-4BAA-8A7A-A850FFA5523D}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:E197"/>
   <sheetViews>
     <sheetView topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A197"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6415,12 +5742,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0079B523-82CE-4ECE-A72D-E8C03BBEEFA7}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7950,12 +7280,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E1538F-A348-4352-B98B-B362DD610648}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E75"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9245,12 +8578,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411032E7-CF4A-43D9-BAB1-7D27C9E6A582}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>